<commit_message>
Updated: March 9, 2022
</commit_message>
<xml_diff>
--- a/raw_data/2022 BAP FX Summary.xlsx
+++ b/raw_data/2022 BAP FX Summary.xlsx
@@ -3,8 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="FEBRUARY" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="JANUARY" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="MARCH" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="FEBRUARY" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="JANUARY" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
   <si>
     <t>TIME</t>
   </si>
@@ -48,6 +49,9 @@
   </si>
   <si>
     <t>FX SETTLEMENT RATE</t>
+  </si>
+  <si>
+    <t>HOLIDAY</t>
   </si>
 </sst>
 </file>
@@ -162,6 +166,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -377,80 +385,80 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
-        <f>workday("02/02/2022",0)</f>
-        <v>44594</v>
+        <f>workday("03/01/2022",0)</f>
+        <v>44621</v>
       </c>
       <c r="C1" s="2">
         <f t="shared" ref="C1:T1" si="1">if(weekday(B1)=6,B1+3,B1+1)</f>
-        <v>44595</v>
+        <v>44622</v>
       </c>
       <c r="D1" s="2">
         <f t="shared" si="1"/>
-        <v>44596</v>
+        <v>44623</v>
       </c>
       <c r="E1" s="2">
         <f t="shared" si="1"/>
-        <v>44599</v>
+        <v>44624</v>
       </c>
       <c r="F1" s="2">
         <f t="shared" si="1"/>
-        <v>44600</v>
+        <v>44627</v>
       </c>
       <c r="G1" s="2">
         <f t="shared" si="1"/>
-        <v>44601</v>
+        <v>44628</v>
       </c>
       <c r="H1" s="2">
         <f t="shared" si="1"/>
-        <v>44602</v>
+        <v>44629</v>
       </c>
       <c r="I1" s="2">
         <f t="shared" si="1"/>
-        <v>44603</v>
+        <v>44630</v>
       </c>
       <c r="J1" s="2">
         <f t="shared" si="1"/>
-        <v>44606</v>
+        <v>44631</v>
       </c>
       <c r="K1" s="2">
         <f t="shared" si="1"/>
-        <v>44607</v>
+        <v>44634</v>
       </c>
       <c r="L1" s="2">
         <f t="shared" si="1"/>
-        <v>44608</v>
+        <v>44635</v>
       </c>
       <c r="M1" s="2">
         <f t="shared" si="1"/>
-        <v>44609</v>
+        <v>44636</v>
       </c>
       <c r="N1" s="2">
         <f t="shared" si="1"/>
-        <v>44610</v>
+        <v>44637</v>
       </c>
       <c r="O1" s="2">
         <f t="shared" si="1"/>
-        <v>44613</v>
+        <v>44638</v>
       </c>
       <c r="P1" s="2">
         <f t="shared" si="1"/>
-        <v>44614</v>
+        <v>44641</v>
       </c>
       <c r="Q1" s="2">
         <f t="shared" si="1"/>
-        <v>44615</v>
+        <v>44642</v>
       </c>
       <c r="R1" s="2">
         <f t="shared" si="1"/>
-        <v>44616</v>
+        <v>44643</v>
       </c>
       <c r="S1" s="2">
         <f t="shared" si="1"/>
-        <v>44617</v>
+        <v>44644</v>
       </c>
       <c r="T1" s="2">
         <f t="shared" si="1"/>
-        <v>44620</v>
+        <v>44645</v>
       </c>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -461,18 +469,26 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>0.3752662037037037</v>
+        <v>0.3759953703703704</v>
       </c>
       <c r="C2" s="4">
-        <v>0.3765162037037037</v>
+        <v>0.3753240740740741</v>
       </c>
       <c r="D2" s="4">
-        <v>0.3771412037037037</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+        <v>0.37971064814814814</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.3754166666666667</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.3753587962962963</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.3751851851851852</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.37528935185185186</v>
+      </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -483,7 +499,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
+      <c r="S2" s="6"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
@@ -494,18 +510,26 @@
         <v>1</v>
       </c>
       <c r="B3" s="6">
-        <v>51.05</v>
+        <v>51.24</v>
       </c>
       <c r="C3" s="6">
-        <v>51.0</v>
+        <v>51.35</v>
       </c>
       <c r="D3" s="6">
-        <v>51.0</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+        <v>51.43</v>
+      </c>
+      <c r="E3" s="6">
+        <v>51.65</v>
+      </c>
+      <c r="F3" s="6">
+        <v>51.9</v>
+      </c>
+      <c r="G3" s="6">
+        <v>52.25</v>
+      </c>
+      <c r="H3" s="6">
+        <v>52.28</v>
+      </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -526,18 +550,26 @@
         <v>2</v>
       </c>
       <c r="B4" s="6">
-        <v>51.18</v>
+        <v>51.295</v>
       </c>
       <c r="C4" s="6">
-        <v>51.1</v>
+        <v>51.455</v>
       </c>
       <c r="D4" s="6">
-        <v>51.14</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+        <v>51.5</v>
+      </c>
+      <c r="E4" s="6">
+        <v>51.75</v>
+      </c>
+      <c r="F4" s="6">
+        <v>52.19</v>
+      </c>
+      <c r="G4" s="6">
+        <v>52.34</v>
+      </c>
+      <c r="H4" s="6">
+        <v>52.31</v>
+      </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -558,18 +590,26 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>50.99</v>
+        <v>51.21</v>
       </c>
       <c r="C5" s="6">
-        <v>50.92</v>
+        <v>51.32</v>
       </c>
       <c r="D5" s="6">
-        <v>50.95</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+        <v>51.42</v>
+      </c>
+      <c r="E5" s="6">
+        <v>51.6</v>
+      </c>
+      <c r="F5" s="6">
+        <v>51.85</v>
+      </c>
+      <c r="G5" s="6">
+        <v>52.01</v>
+      </c>
+      <c r="H5" s="6">
+        <v>52.15</v>
+      </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
@@ -590,18 +630,26 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>51.045</v>
+        <v>51.23</v>
       </c>
       <c r="C6" s="6">
-        <v>51.05</v>
+        <v>51.42</v>
       </c>
       <c r="D6" s="6">
-        <v>51.14</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+        <v>51.5</v>
+      </c>
+      <c r="E6" s="6">
+        <v>51.74</v>
+      </c>
+      <c r="F6" s="6">
+        <v>52.18</v>
+      </c>
+      <c r="G6" s="6">
+        <v>52.32</v>
+      </c>
+      <c r="H6" s="6">
+        <v>52.23</v>
+      </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -622,18 +670,26 @@
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>51.118</v>
+        <v>51.253</v>
       </c>
       <c r="C7" s="6">
-        <v>51.061</v>
+        <v>51.378</v>
       </c>
       <c r="D7" s="6">
-        <v>51.02</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+        <v>51.461</v>
+      </c>
+      <c r="E7" s="6">
+        <v>51.689</v>
+      </c>
+      <c r="F7" s="6">
+        <v>52.001</v>
+      </c>
+      <c r="G7" s="6">
+        <v>52.159</v>
+      </c>
+      <c r="H7" s="6">
+        <v>52.253</v>
+      </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -654,18 +710,26 @@
         <v>6</v>
       </c>
       <c r="B8" s="6">
-        <v>660.86</v>
+        <v>424.67</v>
       </c>
       <c r="C8" s="6">
-        <v>495.0</v>
+        <v>612.0</v>
       </c>
       <c r="D8" s="6">
-        <v>449.0</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+        <v>382.25</v>
+      </c>
+      <c r="E8" s="6">
+        <v>472.22</v>
+      </c>
+      <c r="F8" s="6">
+        <v>908.0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>698.25</v>
+      </c>
+      <c r="H8" s="6">
+        <v>510.92</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -686,18 +750,26 @@
         <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>51.082</v>
+        <v>51.246</v>
       </c>
       <c r="C9" s="6">
-        <v>51.023</v>
+        <v>51.411</v>
       </c>
       <c r="D9" s="6">
-        <v>51.038</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+        <v>51.478</v>
+      </c>
+      <c r="E9" s="6">
+        <v>51.705</v>
+      </c>
+      <c r="F9" s="6">
+        <v>52.141</v>
+      </c>
+      <c r="G9" s="6">
+        <v>52.234</v>
+      </c>
+      <c r="H9" s="6">
+        <v>52.227</v>
+      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -718,18 +790,26 @@
         <v>8</v>
       </c>
       <c r="B10" s="6">
-        <v>526.3</v>
+        <v>517.54</v>
       </c>
       <c r="C10" s="6">
-        <v>557.36</v>
+        <v>420.66</v>
       </c>
       <c r="D10" s="6">
-        <v>443.5</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+        <v>407.13</v>
+      </c>
+      <c r="E10" s="6">
+        <v>321.0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>672.4</v>
+      </c>
+      <c r="G10" s="6">
+        <v>636.5</v>
+      </c>
+      <c r="H10" s="6">
+        <v>624.7</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -750,18 +830,26 @@
         <v>9</v>
       </c>
       <c r="B11" s="6">
-        <v>51.102</v>
+        <v>51.249</v>
       </c>
       <c r="C11" s="6">
-        <v>51.041</v>
+        <v>51.391</v>
       </c>
       <c r="D11" s="6">
-        <v>51.029</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+        <v>51.47</v>
+      </c>
+      <c r="E11" s="6">
+        <v>51.696</v>
+      </c>
+      <c r="F11" s="6">
+        <v>52.061</v>
+      </c>
+      <c r="G11" s="6">
+        <v>52.195</v>
+      </c>
+      <c r="H11" s="6">
+        <v>52.239</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -782,18 +870,26 @@
         <v>10</v>
       </c>
       <c r="B12" s="6">
-        <v>1187.16</v>
+        <v>942.21</v>
       </c>
       <c r="C12" s="6">
-        <v>1052.36</v>
+        <v>1032.66</v>
       </c>
       <c r="D12" s="6">
-        <v>892.5</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+        <v>789.38</v>
+      </c>
+      <c r="E12" s="6">
+        <v>793.22</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1580.4</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1334.75</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1135.62</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -814,18 +910,26 @@
         <v>11</v>
       </c>
       <c r="B13" s="6">
-        <v>51.118</v>
+        <v>51.253</v>
       </c>
       <c r="C13" s="6">
-        <v>51.061</v>
+        <v>51.378</v>
       </c>
       <c r="D13" s="6">
-        <v>51.02</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+        <v>51.461</v>
+      </c>
+      <c r="E13" s="6">
+        <v>51.689</v>
+      </c>
+      <c r="F13" s="6">
+        <v>52.001</v>
+      </c>
+      <c r="G13" s="6">
+        <v>52.159</v>
+      </c>
+      <c r="H13" s="6">
+        <v>52.253</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -901,6 +1005,903 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
+        <f>workday("02/02/2022",0)</f>
+        <v>44594</v>
+      </c>
+      <c r="C1" s="2">
+        <f t="shared" ref="C1:T1" si="1">if(weekday(B1)=6,B1+3,B1+1)</f>
+        <v>44595</v>
+      </c>
+      <c r="D1" s="2">
+        <f t="shared" si="1"/>
+        <v>44596</v>
+      </c>
+      <c r="E1" s="2">
+        <f t="shared" si="1"/>
+        <v>44599</v>
+      </c>
+      <c r="F1" s="2">
+        <f t="shared" si="1"/>
+        <v>44600</v>
+      </c>
+      <c r="G1" s="2">
+        <f t="shared" si="1"/>
+        <v>44601</v>
+      </c>
+      <c r="H1" s="2">
+        <f t="shared" si="1"/>
+        <v>44602</v>
+      </c>
+      <c r="I1" s="2">
+        <f t="shared" si="1"/>
+        <v>44603</v>
+      </c>
+      <c r="J1" s="2">
+        <f t="shared" si="1"/>
+        <v>44606</v>
+      </c>
+      <c r="K1" s="2">
+        <f t="shared" si="1"/>
+        <v>44607</v>
+      </c>
+      <c r="L1" s="2">
+        <f t="shared" si="1"/>
+        <v>44608</v>
+      </c>
+      <c r="M1" s="2">
+        <f t="shared" si="1"/>
+        <v>44609</v>
+      </c>
+      <c r="N1" s="2">
+        <f t="shared" si="1"/>
+        <v>44610</v>
+      </c>
+      <c r="O1" s="2">
+        <f t="shared" si="1"/>
+        <v>44613</v>
+      </c>
+      <c r="P1" s="2">
+        <f t="shared" si="1"/>
+        <v>44614</v>
+      </c>
+      <c r="Q1" s="2">
+        <f t="shared" si="1"/>
+        <v>44615</v>
+      </c>
+      <c r="R1" s="2">
+        <f t="shared" si="1"/>
+        <v>44616</v>
+      </c>
+      <c r="S1" s="2">
+        <f t="shared" si="1"/>
+        <v>44617</v>
+      </c>
+      <c r="T1" s="2">
+        <f t="shared" si="1"/>
+        <v>44620</v>
+      </c>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.3752662037037037</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.3765162037037037</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.3771412037037037</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.3755671296296296</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.3752662037037037</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.37525462962962963</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.37864583333333335</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.37519675925925927</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0.37613425925925925</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0.3784490740740741</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0.3771759259259259</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0.37649305555555557</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0.3801157407407407</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0.3755324074074074</v>
+      </c>
+      <c r="P2" s="4">
+        <v>0.37561342592592595</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>0.37528935185185186</v>
+      </c>
+      <c r="R2" s="4">
+        <v>0.37547453703703704</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="4">
+        <v>0.37754629629629627</v>
+      </c>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>51.05</v>
+      </c>
+      <c r="C3" s="6">
+        <v>51.0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>51.0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>51.25</v>
+      </c>
+      <c r="F3" s="6">
+        <v>51.4</v>
+      </c>
+      <c r="G3" s="6">
+        <v>51.43</v>
+      </c>
+      <c r="H3" s="6">
+        <v>51.3</v>
+      </c>
+      <c r="I3" s="6">
+        <v>51.36</v>
+      </c>
+      <c r="J3" s="6">
+        <v>51.38</v>
+      </c>
+      <c r="K3" s="6">
+        <v>51.36</v>
+      </c>
+      <c r="L3" s="6">
+        <v>51.319</v>
+      </c>
+      <c r="M3" s="7">
+        <v>51.27</v>
+      </c>
+      <c r="N3" s="6">
+        <v>51.34</v>
+      </c>
+      <c r="O3" s="6">
+        <v>51.4</v>
+      </c>
+      <c r="P3" s="6">
+        <v>51.4</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>51.35</v>
+      </c>
+      <c r="R3" s="6">
+        <v>51.18</v>
+      </c>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6">
+        <v>51.39</v>
+      </c>
+      <c r="U3" s="6"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="6"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>51.18</v>
+      </c>
+      <c r="C4" s="6">
+        <v>51.1</v>
+      </c>
+      <c r="D4" s="6">
+        <v>51.14</v>
+      </c>
+      <c r="E4" s="6">
+        <v>51.38</v>
+      </c>
+      <c r="F4" s="6">
+        <v>51.5</v>
+      </c>
+      <c r="G4" s="6">
+        <v>51.445</v>
+      </c>
+      <c r="H4" s="6">
+        <v>51.32</v>
+      </c>
+      <c r="I4" s="6">
+        <v>51.37</v>
+      </c>
+      <c r="J4" s="6">
+        <v>51.405</v>
+      </c>
+      <c r="K4" s="6">
+        <v>51.42</v>
+      </c>
+      <c r="L4" s="6">
+        <v>51.34</v>
+      </c>
+      <c r="M4" s="7">
+        <v>51.36</v>
+      </c>
+      <c r="N4" s="6">
+        <v>51.36</v>
+      </c>
+      <c r="O4" s="6">
+        <v>51.42</v>
+      </c>
+      <c r="P4" s="6">
+        <v>51.48</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>51.365</v>
+      </c>
+      <c r="R4" s="6">
+        <v>51.44</v>
+      </c>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6">
+        <v>51.42</v>
+      </c>
+      <c r="U4" s="6"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="6"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>50.99</v>
+      </c>
+      <c r="C5" s="6">
+        <v>50.92</v>
+      </c>
+      <c r="D5" s="6">
+        <v>50.95</v>
+      </c>
+      <c r="E5" s="6">
+        <v>51.22</v>
+      </c>
+      <c r="F5" s="6">
+        <v>51.38</v>
+      </c>
+      <c r="G5" s="6">
+        <v>51.32</v>
+      </c>
+      <c r="H5" s="6">
+        <v>51.21</v>
+      </c>
+      <c r="I5" s="6">
+        <v>51.29</v>
+      </c>
+      <c r="J5" s="6">
+        <v>51.32</v>
+      </c>
+      <c r="K5" s="6">
+        <v>51.33</v>
+      </c>
+      <c r="L5" s="6">
+        <v>51.27</v>
+      </c>
+      <c r="M5" s="7">
+        <v>51.235</v>
+      </c>
+      <c r="N5" s="6">
+        <v>51.28</v>
+      </c>
+      <c r="O5" s="6">
+        <v>51.36</v>
+      </c>
+      <c r="P5" s="6">
+        <v>51.4</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>51.1</v>
+      </c>
+      <c r="R5" s="6">
+        <v>51.17</v>
+      </c>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6">
+        <v>51.265</v>
+      </c>
+      <c r="U5" s="6"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="6"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
+        <v>51.045</v>
+      </c>
+      <c r="C6" s="6">
+        <v>51.05</v>
+      </c>
+      <c r="D6" s="6">
+        <v>51.14</v>
+      </c>
+      <c r="E6" s="6">
+        <v>51.37</v>
+      </c>
+      <c r="F6" s="6">
+        <v>51.5</v>
+      </c>
+      <c r="G6" s="6">
+        <v>51.34</v>
+      </c>
+      <c r="H6" s="6">
+        <v>51.235</v>
+      </c>
+      <c r="I6" s="6">
+        <v>51.34</v>
+      </c>
+      <c r="J6" s="6">
+        <v>51.37</v>
+      </c>
+      <c r="K6" s="6">
+        <v>51.382</v>
+      </c>
+      <c r="L6" s="6">
+        <v>51.285</v>
+      </c>
+      <c r="M6" s="7">
+        <v>51.33</v>
+      </c>
+      <c r="N6" s="6">
+        <v>51.35</v>
+      </c>
+      <c r="O6" s="6">
+        <v>51.38</v>
+      </c>
+      <c r="P6" s="6">
+        <v>51.45</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>51.1</v>
+      </c>
+      <c r="R6" s="6">
+        <v>51.34</v>
+      </c>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6">
+        <v>51.27</v>
+      </c>
+      <c r="U6" s="6"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="6"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
+        <v>51.118</v>
+      </c>
+      <c r="C7" s="6">
+        <v>51.061</v>
+      </c>
+      <c r="D7" s="6">
+        <v>51.02</v>
+      </c>
+      <c r="E7" s="6">
+        <v>51.282</v>
+      </c>
+      <c r="F7" s="6">
+        <v>51.417</v>
+      </c>
+      <c r="G7" s="6">
+        <v>51.386</v>
+      </c>
+      <c r="H7" s="6">
+        <v>51.279</v>
+      </c>
+      <c r="I7" s="6">
+        <v>51.329</v>
+      </c>
+      <c r="J7" s="6">
+        <v>51.386</v>
+      </c>
+      <c r="K7" s="6">
+        <v>51.371</v>
+      </c>
+      <c r="L7" s="6">
+        <v>51.304</v>
+      </c>
+      <c r="M7" s="7">
+        <v>51.267</v>
+      </c>
+      <c r="N7" s="6">
+        <v>51.315</v>
+      </c>
+      <c r="O7" s="6">
+        <v>51.393</v>
+      </c>
+      <c r="P7" s="6">
+        <v>51.445</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>51.338</v>
+      </c>
+      <c r="R7" s="6">
+        <v>51.237</v>
+      </c>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6">
+        <v>51.399</v>
+      </c>
+      <c r="U7" s="6"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="6"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
+        <v>660.86</v>
+      </c>
+      <c r="C8" s="6">
+        <v>495.0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>449.0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>500.0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>487.0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>592.0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>452.0</v>
+      </c>
+      <c r="I8" s="6">
+        <v>497.0</v>
+      </c>
+      <c r="J8" s="6">
+        <v>329.5</v>
+      </c>
+      <c r="K8" s="6">
+        <v>291.28</v>
+      </c>
+      <c r="L8" s="6">
+        <v>352.0</v>
+      </c>
+      <c r="M8" s="7">
+        <v>385.3</v>
+      </c>
+      <c r="N8" s="6">
+        <v>263.2</v>
+      </c>
+      <c r="O8" s="6">
+        <v>368.0</v>
+      </c>
+      <c r="P8" s="6">
+        <v>390.5</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>404.8</v>
+      </c>
+      <c r="R8" s="6">
+        <v>539.2</v>
+      </c>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6">
+        <v>467.0</v>
+      </c>
+      <c r="U8" s="6"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="6"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6">
+        <v>51.082</v>
+      </c>
+      <c r="C9" s="6">
+        <v>51.023</v>
+      </c>
+      <c r="D9" s="6">
+        <v>51.038</v>
+      </c>
+      <c r="E9" s="6">
+        <v>51.305</v>
+      </c>
+      <c r="F9" s="6">
+        <v>51.453</v>
+      </c>
+      <c r="G9" s="6">
+        <v>51.363</v>
+      </c>
+      <c r="H9" s="6">
+        <v>51.255</v>
+      </c>
+      <c r="I9" s="6">
+        <v>51.329</v>
+      </c>
+      <c r="J9" s="6">
+        <v>51.362</v>
+      </c>
+      <c r="K9" s="6">
+        <v>51.368</v>
+      </c>
+      <c r="L9" s="6">
+        <v>51.284</v>
+      </c>
+      <c r="M9" s="7">
+        <v>51.306</v>
+      </c>
+      <c r="N9" s="6">
+        <v>51.314</v>
+      </c>
+      <c r="O9" s="6">
+        <v>51.393</v>
+      </c>
+      <c r="P9" s="6">
+        <v>51.445</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>51.22</v>
+      </c>
+      <c r="R9" s="6">
+        <v>51.339</v>
+      </c>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6">
+        <v>51.364</v>
+      </c>
+      <c r="U9" s="6"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="6"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6">
+        <v>526.3</v>
+      </c>
+      <c r="C10" s="6">
+        <v>557.36</v>
+      </c>
+      <c r="D10" s="6">
+        <v>443.5</v>
+      </c>
+      <c r="E10" s="6">
+        <v>459.3</v>
+      </c>
+      <c r="F10" s="6">
+        <v>518.1</v>
+      </c>
+      <c r="G10" s="6">
+        <v>400.1</v>
+      </c>
+      <c r="H10" s="6">
+        <v>485.4</v>
+      </c>
+      <c r="I10" s="6">
+        <v>416.88</v>
+      </c>
+      <c r="J10" s="6">
+        <v>297.5</v>
+      </c>
+      <c r="K10" s="6">
+        <v>269.0</v>
+      </c>
+      <c r="L10" s="6">
+        <v>244.1</v>
+      </c>
+      <c r="M10" s="7">
+        <v>439.1</v>
+      </c>
+      <c r="N10" s="6">
+        <v>283.0</v>
+      </c>
+      <c r="O10" s="6">
+        <v>345.5</v>
+      </c>
+      <c r="P10" s="6">
+        <v>391.9</v>
+      </c>
+      <c r="Q10" s="12">
+        <v>529.4</v>
+      </c>
+      <c r="R10" s="6">
+        <v>620.9</v>
+      </c>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6">
+        <v>313.5</v>
+      </c>
+      <c r="U10" s="6"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="6"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6">
+        <v>51.102</v>
+      </c>
+      <c r="C11" s="6">
+        <v>51.041</v>
+      </c>
+      <c r="D11" s="6">
+        <v>51.029</v>
+      </c>
+      <c r="E11" s="6">
+        <v>51.293</v>
+      </c>
+      <c r="F11" s="6">
+        <v>51.436</v>
+      </c>
+      <c r="G11" s="6">
+        <v>51.377</v>
+      </c>
+      <c r="H11" s="6">
+        <v>51.267</v>
+      </c>
+      <c r="I11" s="6">
+        <v>51.329</v>
+      </c>
+      <c r="J11" s="6">
+        <v>51.375</v>
+      </c>
+      <c r="K11" s="6">
+        <v>51.37</v>
+      </c>
+      <c r="L11" s="6">
+        <v>51.296</v>
+      </c>
+      <c r="M11" s="7">
+        <v>51.288</v>
+      </c>
+      <c r="N11" s="6">
+        <v>51.314</v>
+      </c>
+      <c r="O11" s="6">
+        <v>51.393</v>
+      </c>
+      <c r="P11" s="6">
+        <v>51.445</v>
+      </c>
+      <c r="Q11" s="12">
+        <v>51.271</v>
+      </c>
+      <c r="R11" s="6">
+        <v>51.291</v>
+      </c>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6">
+        <v>51.385</v>
+      </c>
+      <c r="U11" s="6"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="6"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1187.16</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1052.36</v>
+      </c>
+      <c r="D12" s="6">
+        <v>892.5</v>
+      </c>
+      <c r="E12" s="6">
+        <v>959.3</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1005.1</v>
+      </c>
+      <c r="G12" s="6">
+        <v>992.1</v>
+      </c>
+      <c r="H12" s="6">
+        <v>937.4</v>
+      </c>
+      <c r="I12" s="6">
+        <v>913.88</v>
+      </c>
+      <c r="J12" s="6">
+        <v>627.0</v>
+      </c>
+      <c r="K12" s="6">
+        <v>560.28</v>
+      </c>
+      <c r="L12" s="6">
+        <v>596.1</v>
+      </c>
+      <c r="M12" s="7">
+        <v>824.4</v>
+      </c>
+      <c r="N12" s="6">
+        <v>546.2</v>
+      </c>
+      <c r="O12" s="6">
+        <v>713.5</v>
+      </c>
+      <c r="P12" s="6">
+        <v>782.4</v>
+      </c>
+      <c r="Q12" s="12">
+        <v>934.2</v>
+      </c>
+      <c r="R12" s="6">
+        <v>1160.1</v>
+      </c>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6">
+        <v>780.5</v>
+      </c>
+      <c r="U12" s="6"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="6"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6">
+        <v>51.118</v>
+      </c>
+      <c r="C13" s="6">
+        <v>51.061</v>
+      </c>
+      <c r="D13" s="6">
+        <v>51.02</v>
+      </c>
+      <c r="E13" s="6">
+        <v>51.282</v>
+      </c>
+      <c r="F13" s="6">
+        <v>51.417</v>
+      </c>
+      <c r="G13" s="6">
+        <v>51.386</v>
+      </c>
+      <c r="H13" s="6">
+        <v>51.279</v>
+      </c>
+      <c r="I13" s="6">
+        <v>51.329</v>
+      </c>
+      <c r="J13" s="6">
+        <v>51.386</v>
+      </c>
+      <c r="K13" s="6">
+        <v>51.371</v>
+      </c>
+      <c r="L13" s="6">
+        <v>51.304</v>
+      </c>
+      <c r="M13" s="6">
+        <v>51.267</v>
+      </c>
+      <c r="N13" s="6">
+        <v>51.315</v>
+      </c>
+      <c r="O13" s="6">
+        <v>51.393</v>
+      </c>
+      <c r="P13" s="6">
+        <v>51.445</v>
+      </c>
+      <c r="Q13" s="12">
+        <v>51.338</v>
+      </c>
+      <c r="R13" s="6">
+        <v>51.237</v>
+      </c>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6">
+        <v>51.399</v>
+      </c>
+      <c r="U13" s="6"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="6"/>
+    </row>
+    <row r="15">
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16">
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17">
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20">
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21">
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22">
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="V2:V13">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(V2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1" pane="topRight"/>
+      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
+      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2">
         <f>workday("01/03/2022",0)</f>
         <v>44564</v>
       </c>

</xml_diff>

<commit_message>
updated as of Dec. 28, 2022
</commit_message>
<xml_diff>
--- a/raw_data/2022 BAP FX Summary.xlsx
+++ b/raw_data/2022 BAP FX Summary.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="20">
   <si>
     <t>TIME</t>
   </si>
@@ -635,10 +635,18 @@
       <c r="Q2" s="3">
         <v>0.3751157407407407</v>
       </c>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
+      <c r="R2" s="3">
+        <v>0.37527777777777777</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0.3762847222222222</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0.3762847222222222</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -689,6 +697,15 @@
       <c r="Q3" s="4">
         <v>55.045</v>
       </c>
+      <c r="R3" s="4">
+        <v>55.25</v>
+      </c>
+      <c r="T3" s="4">
+        <v>55.15</v>
+      </c>
+      <c r="U3" s="4">
+        <v>55.9</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
@@ -739,6 +756,15 @@
       <c r="Q4" s="4">
         <v>55.18</v>
       </c>
+      <c r="R4" s="4">
+        <v>55.35</v>
+      </c>
+      <c r="T4" s="4">
+        <v>55.93</v>
+      </c>
+      <c r="U4" s="4">
+        <v>56.3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
@@ -789,6 +815,15 @@
       <c r="Q5" s="4">
         <v>55.045</v>
       </c>
+      <c r="R5" s="4">
+        <v>55.15</v>
+      </c>
+      <c r="T5" s="4">
+        <v>55.15</v>
+      </c>
+      <c r="U5" s="4">
+        <v>55.89</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
@@ -839,6 +874,15 @@
       <c r="Q6" s="4">
         <v>55.09</v>
       </c>
+      <c r="R6" s="4">
+        <v>55.15</v>
+      </c>
+      <c r="T6" s="4">
+        <v>55.9</v>
+      </c>
+      <c r="U6" s="4">
+        <v>56.2</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
@@ -889,6 +933,15 @@
       <c r="Q7" s="4">
         <v>55.135</v>
       </c>
+      <c r="R7" s="4">
+        <v>55.263</v>
+      </c>
+      <c r="T7" s="4">
+        <v>55.278</v>
+      </c>
+      <c r="U7" s="4">
+        <v>56.106</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
@@ -939,6 +992,15 @@
       <c r="Q8" s="4">
         <v>557.9</v>
       </c>
+      <c r="R8" s="4">
+        <v>532.44</v>
+      </c>
+      <c r="T8" s="4">
+        <v>520.87</v>
+      </c>
+      <c r="U8" s="4">
+        <v>566.25</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
@@ -989,6 +1051,15 @@
       <c r="Q9" s="4">
         <v>55.118</v>
       </c>
+      <c r="R9" s="4">
+        <v>55.28</v>
+      </c>
+      <c r="T9" s="4">
+        <v>55.596</v>
+      </c>
+      <c r="U9" s="4">
+        <v>56.144</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
@@ -1039,6 +1110,15 @@
       <c r="Q10" s="4">
         <v>216.3</v>
       </c>
+      <c r="R10" s="4">
+        <v>487.6</v>
+      </c>
+      <c r="T10" s="4">
+        <v>292.4</v>
+      </c>
+      <c r="U10" s="4">
+        <v>316.6</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
@@ -1089,6 +1169,15 @@
       <c r="Q11" s="4">
         <v>55.13</v>
       </c>
+      <c r="R11" s="4">
+        <v>55.271</v>
+      </c>
+      <c r="T11" s="4">
+        <v>55.393</v>
+      </c>
+      <c r="U11" s="4">
+        <v>56.12</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
@@ -1139,6 +1228,15 @@
       <c r="Q12" s="4">
         <v>774.2</v>
       </c>
+      <c r="R12" s="4">
+        <v>1020.04</v>
+      </c>
+      <c r="T12" s="4">
+        <v>813.27</v>
+      </c>
+      <c r="U12" s="4">
+        <v>882.85</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
@@ -1188,6 +1286,15 @@
       </c>
       <c r="Q13" s="4">
         <v>55.135</v>
+      </c>
+      <c r="R13" s="4">
+        <v>55.263</v>
+      </c>
+      <c r="T13" s="4">
+        <v>55.278</v>
+      </c>
+      <c r="U13" s="4">
+        <v>56.106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated as of Feb. 10, 2023
</commit_message>
<xml_diff>
--- a/raw_data/2022 BAP FX Summary.xlsx
+++ b/raw_data/2022 BAP FX Summary.xlsx
@@ -647,6 +647,9 @@
       <c r="U2" s="3">
         <v>0.3762847222222222</v>
       </c>
+      <c r="V2" s="3">
+        <v>0.37636574074074075</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -706,6 +709,9 @@
       <c r="U3" s="4">
         <v>55.9</v>
       </c>
+      <c r="V3" s="4">
+        <v>56.17</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
@@ -765,6 +771,9 @@
       <c r="U4" s="4">
         <v>56.3</v>
       </c>
+      <c r="V4" s="4">
+        <v>56.18</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
@@ -824,6 +833,9 @@
       <c r="U5" s="4">
         <v>55.89</v>
       </c>
+      <c r="V5" s="4">
+        <v>55.67</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
@@ -883,6 +895,9 @@
       <c r="U6" s="4">
         <v>56.2</v>
       </c>
+      <c r="V6" s="4">
+        <v>55.755</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
@@ -942,6 +957,9 @@
       <c r="U7" s="4">
         <v>56.106</v>
       </c>
+      <c r="V7" s="4">
+        <v>55.818</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
@@ -1001,6 +1019,9 @@
       <c r="U8" s="4">
         <v>566.25</v>
       </c>
+      <c r="V8" s="4">
+        <v>431.7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
@@ -1060,6 +1081,9 @@
       <c r="U9" s="4">
         <v>56.144</v>
       </c>
+      <c r="V9" s="4">
+        <v>55.811</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
@@ -1119,6 +1143,9 @@
       <c r="U10" s="4">
         <v>316.6</v>
       </c>
+      <c r="V10" s="4">
+        <v>376.1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
@@ -1178,6 +1205,9 @@
       <c r="U11" s="4">
         <v>56.12</v>
       </c>
+      <c r="V11" s="4">
+        <v>55.815</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
@@ -1237,6 +1267,9 @@
       <c r="U12" s="4">
         <v>882.85</v>
       </c>
+      <c r="V12" s="4">
+        <v>807.8</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
@@ -1295,6 +1328,9 @@
       </c>
       <c r="U13" s="4">
         <v>56.106</v>
+      </c>
+      <c r="V13" s="4">
+        <v>55.818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>